<commit_message>
feat: add usedata to be able to compare BMF methods in another vignette
</commit_message>
<xml_diff>
--- a/vignettes/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
+++ b/vignettes/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -378,41 +378,6 @@
           <t>max</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>chem_label</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>family</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sub_family_TAG</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sub_family_name</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>logKow</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>n_C</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>LOQ_biote</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -429,24 +394,6 @@
       <c r="D2">
         <v>19.38</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CB-101</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="I2">
-        <v>6.38</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -463,24 +410,6 @@
       <c r="D3">
         <v>10.01</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>CB-105</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="I3">
-        <v>6.65</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -497,24 +426,6 @@
       <c r="D4">
         <v>20.75</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>CB-110</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="I4">
-        <v>6.48</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -531,24 +442,6 @@
       <c r="D5">
         <v>6.1</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>CB-118</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>penta-CB</t>
-        </is>
-      </c>
-      <c r="I5">
-        <v>6.74</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -565,24 +458,6 @@
       <c r="D6">
         <v>26.53</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CB-128</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="I6">
-        <v>6.74</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -599,24 +474,6 @@
       <c r="D7">
         <v>16.04</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CB-132</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="I7">
-        <v>6.58</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -633,24 +490,6 @@
       <c r="D8">
         <v>10.85</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>CB-138</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="I8">
-        <v>6.83</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -667,24 +506,6 @@
       <c r="D9">
         <v>14.14</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>CB-149</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="I9">
-        <v>6.67</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -701,24 +522,6 @@
       <c r="D10">
         <v>9.25</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>CB-153</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="I10">
-        <v>6.92</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -735,24 +538,6 @@
       <c r="D11">
         <v>3.85</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>CB-156</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>hexa-CB</t>
-        </is>
-      </c>
-      <c r="I11">
-        <v>7.18</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -769,24 +554,6 @@
       <c r="D12">
         <v>4</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>CB-170</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>hepta-CB</t>
-        </is>
-      </c>
-      <c r="I12">
-        <v>7.11</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -803,24 +570,6 @@
       <c r="D13">
         <v>7.58</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>CB-180</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>hepta-CB</t>
-        </is>
-      </c>
-      <c r="I13">
-        <v>7.36</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -837,24 +586,6 @@
       <c r="D14">
         <v>2.64</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>CB-028</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>tri-CB</t>
-        </is>
-      </c>
-      <c r="I14">
-        <v>5.67</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -871,24 +602,6 @@
       <c r="D15">
         <v>1.76</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>CB-031</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>tri-CB</t>
-        </is>
-      </c>
-      <c r="I15">
-        <v>5.67</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -905,24 +618,6 @@
       <c r="D16">
         <v>6.22</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CB-044</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>tetra-CB</t>
-        </is>
-      </c>
-      <c r="I16">
-        <v>5.75</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -939,24 +634,6 @@
       <c r="D17">
         <v>7.64</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>CB-049</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>tetra-CB</t>
-        </is>
-      </c>
-      <c r="I17">
-        <v>5.63</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -973,23 +650,21 @@
       <c r="D18">
         <v>4.08</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>CB-052</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>PCB</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>tetra-CB</t>
-        </is>
-      </c>
-      <c r="I18">
-        <v>5.84</v>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sumPCB</t>
+        </is>
+      </c>
+      <c r="B19">
+        <v>0.2</v>
+      </c>
+      <c r="C19">
+        <v>1.22</v>
+      </c>
+      <c r="D19">
+        <v>6.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: reorder PCB congeners in data and graphs
</commit_message>
<xml_diff>
--- a/vignettes/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
+++ b/vignettes/results/BMF_computation_PCB_ng_glw/1.BMF_species_PCB_ng_glw_summarised.xlsx
@@ -382,289 +382,289 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CB101</t>
+          <t>sumPCB</t>
         </is>
       </c>
       <c r="B2">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
-        <v>1.9</v>
+        <v>1.22</v>
       </c>
       <c r="D2">
-        <v>19.38</v>
+        <v>6.49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CB105</t>
+          <t>CB28</t>
         </is>
       </c>
       <c r="B3">
-        <v>0.21</v>
+        <v>0.06</v>
       </c>
       <c r="C3">
-        <v>1.36</v>
+        <v>0.6</v>
       </c>
       <c r="D3">
-        <v>10.01</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CB110</t>
+          <t>CB31</t>
         </is>
       </c>
       <c r="B4">
-        <v>0.14</v>
+        <v>0.01</v>
       </c>
       <c r="C4">
-        <v>1.86</v>
+        <v>0.31</v>
       </c>
       <c r="D4">
-        <v>20.75</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CB118</t>
+          <t>CB44</t>
         </is>
       </c>
       <c r="B5">
-        <v>0.22</v>
+        <v>0.09</v>
       </c>
       <c r="C5">
-        <v>1.35</v>
+        <v>0.92</v>
       </c>
       <c r="D5">
-        <v>6.1</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CB128</t>
+          <t>CB49</t>
         </is>
       </c>
       <c r="B6">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
-        <v>2.34</v>
+        <v>1.03</v>
       </c>
       <c r="D6">
-        <v>26.53</v>
+        <v>7.64</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CB132</t>
+          <t>CB52</t>
         </is>
       </c>
       <c r="B7">
         <v>0.12</v>
       </c>
       <c r="C7">
-        <v>1.33</v>
+        <v>1.22</v>
       </c>
       <c r="D7">
-        <v>16.04</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CB138</t>
+          <t>CB101</t>
         </is>
       </c>
       <c r="B8">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C8">
-        <v>1.29</v>
+        <v>1.9</v>
       </c>
       <c r="D8">
-        <v>10.85</v>
+        <v>19.38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CB149</t>
+          <t>CB105</t>
         </is>
       </c>
       <c r="B9">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="C9">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="D9">
-        <v>14.14</v>
+        <v>10.01</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CB153</t>
+          <t>CB110</t>
         </is>
       </c>
       <c r="B10">
-        <v>0.22</v>
+        <v>0.14</v>
       </c>
       <c r="C10">
-        <v>1.41</v>
+        <v>1.86</v>
       </c>
       <c r="D10">
-        <v>9.25</v>
+        <v>20.75</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CB156</t>
+          <t>CB118</t>
         </is>
       </c>
       <c r="B11">
         <v>0.22</v>
       </c>
       <c r="C11">
-        <v>1.02</v>
+        <v>1.35</v>
       </c>
       <c r="D11">
-        <v>3.85</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CB170</t>
+          <t>CB128</t>
         </is>
       </c>
       <c r="B12">
-        <v>0.28</v>
+        <v>0.24</v>
       </c>
       <c r="C12">
-        <v>1.16</v>
+        <v>2.34</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>26.53</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CB180</t>
+          <t>CB132</t>
         </is>
       </c>
       <c r="B13">
-        <v>0.28</v>
+        <v>0.12</v>
       </c>
       <c r="C13">
-        <v>1.62</v>
+        <v>1.33</v>
       </c>
       <c r="D13">
-        <v>7.58</v>
+        <v>16.04</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CB28</t>
+          <t>CB138</t>
         </is>
       </c>
       <c r="B14">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>1.29</v>
       </c>
       <c r="D14">
-        <v>2.64</v>
+        <v>10.85</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CB31</t>
+          <t>CB149</t>
         </is>
       </c>
       <c r="B15">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
       <c r="C15">
-        <v>0.31</v>
+        <v>1.35</v>
       </c>
       <c r="D15">
-        <v>1.76</v>
+        <v>14.14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CB44</t>
+          <t>CB153</t>
         </is>
       </c>
       <c r="B16">
-        <v>0.09</v>
+        <v>0.22</v>
       </c>
       <c r="C16">
-        <v>0.92</v>
+        <v>1.41</v>
       </c>
       <c r="D16">
-        <v>6.22</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CB49</t>
+          <t>CB156</t>
         </is>
       </c>
       <c r="B17">
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="C17">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="D17">
-        <v>7.64</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CB52</t>
+          <t>CB170</t>
         </is>
       </c>
       <c r="B18">
-        <v>0.12</v>
+        <v>0.28</v>
       </c>
       <c r="C18">
-        <v>1.22</v>
+        <v>1.16</v>
       </c>
       <c r="D18">
-        <v>4.08</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>sumPCB</t>
+          <t>CB180</t>
         </is>
       </c>
       <c r="B19">
-        <v>0.2</v>
+        <v>0.28</v>
       </c>
       <c r="C19">
-        <v>1.22</v>
+        <v>1.62</v>
       </c>
       <c r="D19">
-        <v>6.49</v>
+        <v>7.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>